<commit_message>
Adds public and private results and updates interactions markdown.
</commit_message>
<xml_diff>
--- a/source_emails/form_outcomes_final.xlsx
+++ b/source_emails/form_outcomes_final.xlsx
@@ -514,7 +514,7 @@
     <t>x</t>
   </si>
   <si>
-    <t>ST</t>
+    <t>Overall STDEV</t>
   </si>
 </sst>
 </file>
@@ -1488,11 +1488,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-719582816"/>
-        <c:axId val="-759051456"/>
+        <c:axId val="119159152"/>
+        <c:axId val="118346592"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-719582816"/>
+        <c:axId val="119159152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1590,12 +1590,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-759051456"/>
+        <c:crossAx val="118346592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-759051456"/>
+        <c:axId val="118346592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1688,7 +1688,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-719582816"/>
+        <c:crossAx val="119159152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2565,11 +2565,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-756195216"/>
-        <c:axId val="-756191456"/>
+        <c:axId val="119195920"/>
+        <c:axId val="119199680"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-756195216"/>
+        <c:axId val="119195920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2667,12 +2667,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-756191456"/>
+        <c:crossAx val="119199680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-756191456"/>
+        <c:axId val="119199680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2764,7 +2764,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-756195216"/>
+        <c:crossAx val="119195920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3635,11 +3635,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-758871120"/>
-        <c:axId val="-758919712"/>
+        <c:axId val="119233440"/>
+        <c:axId val="119237200"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-758871120"/>
+        <c:axId val="119233440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3737,12 +3737,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-758919712"/>
+        <c:crossAx val="119237200"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-758919712"/>
+        <c:axId val="119237200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3834,7 +3834,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-758871120"/>
+        <c:crossAx val="119233440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4705,11 +4705,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-719518608"/>
-        <c:axId val="-719514848"/>
+        <c:axId val="119262272"/>
+        <c:axId val="119266032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-719518608"/>
+        <c:axId val="119262272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4807,12 +4807,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-719514848"/>
+        <c:crossAx val="119266032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-719514848"/>
+        <c:axId val="119266032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4905,7 +4905,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-719518608"/>
+        <c:crossAx val="119262272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5758,11 +5758,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-719512368"/>
-        <c:axId val="-719509024"/>
+        <c:axId val="82408496"/>
+        <c:axId val="82414032"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-719512368"/>
+        <c:axId val="82408496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5860,12 +5860,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-719509024"/>
+        <c:crossAx val="82414032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-719509024"/>
+        <c:axId val="82414032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5958,7 +5958,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-719512368"/>
+        <c:crossAx val="82408496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9180,8 +9180,8 @@
   <dimension ref="A1:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H67" sqref="H67"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C79" sqref="C79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>